<commit_message>
laptop pre explosion backup
puter plugged into the xds110 thats connected to masterboard_A 1.0 . it only shares a ground but god save this laptop if the mcu gives out for some reason
</commit_message>
<xml_diff>
--- a/hardware/MasterBoard_A/Meta MasterBoard A.xlsx
+++ b/hardware/MasterBoard_A/Meta MasterBoard A.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="175">
   <si>
     <t xml:space="preserve">last updated</t>
   </si>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">A7</t>
   </si>
   <si>
-    <t xml:space="preserve">lable connector pins</t>
+    <t xml:space="preserve">lable connector pins, especially the uart pinout</t>
   </si>
   <si>
     <t xml:space="preserve">A8</t>
@@ -238,13 +238,25 @@
     <t xml:space="preserve">A10</t>
   </si>
   <si>
+    <t xml:space="preserve">uart pins too close to jtag(“actually its a swd connection”🤓) header. Connector plastic like 0.5mm from touching uart pin, cannot put dupont on uart :(</t>
+  </si>
+  <si>
     <t xml:space="preserve">A11</t>
   </si>
   <si>
+    <t xml:space="preserve">make HRLV connector a 2x3 molex, to match what the voltage tap has</t>
+  </si>
+  <si>
     <t xml:space="preserve">A12</t>
   </si>
   <si>
+    <t xml:space="preserve">interlog use constant current source, not pull up. Like 120mA max CC from HRLV sounds enough</t>
+  </si>
+  <si>
     <t xml:space="preserve">A13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check thermals over long runtime</t>
   </si>
   <si>
     <t xml:space="preserve">A14</t>
@@ -1017,8 +1029,8 @@
   </sheetPr>
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S16" activeCellId="0" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1274,7 +1286,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1334,7 +1346,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1350,8 +1362,11 @@
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L12, $G$15:$G$1000, 0)), "n/a")</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1361,14 +1376,17 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M13" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L13, $G$15:$G$1000, 0)), "n/a")</f>
         <v>n/a</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1378,25 +1396,31 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M14" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L14, $G$15:$G$1000, 0)), "n/a")</f>
         <v>spi0 SCLK</v>
       </c>
+      <c r="S14" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L15" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M15" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L15, $G$15:$G$1000, 0)), "n/a")</f>
         <v>spi0 MISO/POCI</v>
       </c>
+      <c r="S15" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L16" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="M16" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L16, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1405,7 +1429,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1415,7 +1439,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="L17" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="M17" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L17, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1424,19 +1448,19 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
@@ -1444,7 +1468,7 @@
       </c>
       <c r="H18" s="6"/>
       <c r="L18" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="M18" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L18, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1459,13 +1483,13 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M19" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L19, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1480,21 +1504,21 @@
         <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
       <c r="G20" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M20" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L20, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1508,18 +1532,18 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
       <c r="G21" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M21" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L21, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1533,18 +1557,18 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
       <c r="G22" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="M22" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L22, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1558,18 +1582,18 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
       <c r="G23" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="M23" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L23, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1583,18 +1607,18 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
       <c r="G24" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M24" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L24, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1608,18 +1632,18 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="M25" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L25, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1633,18 +1657,18 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="M26" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L26, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1656,24 +1680,24 @@
         <v>33</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="M27" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L27, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1685,24 +1709,24 @@
         <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="M28" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L28, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1711,27 +1735,27 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M29" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L29, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1740,27 +1764,27 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="M30" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L30, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1769,7 +1793,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L31" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="M31" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L31, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1778,7 +1802,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1788,7 +1812,7 @@
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="L32" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="M32" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L32, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1803,13 +1827,13 @@
         <v>15</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
@@ -1817,7 +1841,7 @@
       </c>
       <c r="H33" s="6"/>
       <c r="L33" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="M33" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L33, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1832,13 +1856,13 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M34" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L34, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1850,26 +1874,26 @@
         <v>27</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="M35" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L35, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1881,26 +1905,26 @@
         <v>27</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="M36" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L36, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1912,26 +1936,26 @@
         <v>27</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="M37" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L37, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1943,26 +1967,26 @@
         <v>27</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M38" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L38, $G$15:$G$1000, 0)), "n/a")</f>
@@ -1974,24 +1998,24 @@
         <v>27</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="M39" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L39, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2003,13 +2027,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -2017,10 +2041,10 @@
         <v>37</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M40" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L40, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2032,13 +2056,13 @@
         <v>27</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -2046,10 +2070,10 @@
         <v>44</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="M41" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L41, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2061,24 +2085,24 @@
         <v>27</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="M42" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L42, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2090,24 +2114,24 @@
         <v>27</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
       <c r="G43" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="M43" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L43, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2119,24 +2143,24 @@
         <v>27</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="M44" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L44, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2148,24 +2172,24 @@
         <v>27</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="M45" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L45, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2177,26 +2201,26 @@
         <v>27</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H46" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="L46" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M46" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L46, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2208,26 +2232,26 @@
         <v>27</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F47" s="10"/>
       <c r="G47" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="H47" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="L47" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="M47" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L47, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2239,26 +2263,26 @@
         <v>27</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="L48" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="M48" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L48, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2270,24 +2294,24 @@
         <v>27</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="M49" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L49, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2299,26 +2323,26 @@
         <v>27</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F50" s="10"/>
       <c r="G50" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="M50" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L50, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2330,26 +2354,26 @@
         <v>27</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F51" s="10"/>
       <c r="G51" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="M51" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L51, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2361,24 +2385,24 @@
         <v>27</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="M52" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L52, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2393,21 +2417,21 @@
         <v>39</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="M53" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L53, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2422,21 +2446,21 @@
         <v>39</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="M54" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L54, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2453,7 +2477,7 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="L55" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="M55" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L55, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2470,7 +2494,7 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="L56" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M56" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L56, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2487,7 +2511,7 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="L57" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="M57" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L57, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2504,7 +2528,7 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="L58" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="M58" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L58, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2513,7 +2537,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L59" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="M59" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L59, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2522,7 +2546,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L60" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="M60" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L60, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2531,7 +2555,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L61" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="M61" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L61, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2540,7 +2564,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L62" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="M62" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L62, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2549,7 +2573,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L63" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="M63" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L63, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2558,7 +2582,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L64" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="M64" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L64, $G$15:$G$1000, 0)), "n/a")</f>
@@ -2567,7 +2591,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L65" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M65" s="3" t="str">
         <f aca="false">IFERROR(INDEX($H$15:$H$1000, MATCH($L65, $G$15:$G$1000, 0)), "n/a")</f>

</xml_diff>

<commit_message>
mb 1.1 on da way. more shuffling
trying to be more professional about the part choices. obtuse excel sheet of pain has arrived.
</commit_message>
<xml_diff>
--- a/hardware/MasterBoard_A/Meta MasterBoard A.xlsx
+++ b/hardware/MasterBoard_A/Meta MasterBoard A.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\BeeMS\hardware\MasterBoard_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D816DD99-A8B6-4B4C-AABD-5B18803C7311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E02431-BFA1-4281-9FAB-E97B2003C929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="1.0 routing" sheetId="1" r:id="rId1"/>
     <sheet name="1.1" sheetId="2" r:id="rId2"/>
+    <sheet name="1.1 power" sheetId="3" r:id="rId3"/>
+    <sheet name="1.1 routing" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -92,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="218">
   <si>
     <t>last updated</t>
   </si>
@@ -676,28 +678,76 @@
     <t>corrected w5500 layout and oscillator choice with tested design from "W5500 testing" project</t>
   </si>
   <si>
-    <t>added UV proteciton for sheet "PWM sig bank 1"</t>
-  </si>
-  <si>
     <t>nuh uh</t>
   </si>
   <si>
-    <t>todo before</t>
-  </si>
-  <si>
-    <t>expand PWM sig bank 1</t>
-  </si>
-  <si>
-    <t>test the sig bank</t>
-  </si>
-  <si>
     <t>molex connector for da ethernet :skull: to get around the hv rated cable wire rule</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>dim indicator leds. Changed load resistor from 2.4k to 3.32k</t>
+  </si>
+  <si>
+    <t>LV batt</t>
+  </si>
+  <si>
+    <t>GLV PSU</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>designator</t>
+  </si>
+  <si>
+    <t>sheet name</t>
+  </si>
+  <si>
+    <t>default sheet name</t>
+  </si>
+  <si>
+    <t>PWM sig bank</t>
+  </si>
+  <si>
+    <t>Analog Fault Failsafe</t>
+  </si>
+  <si>
+    <t>Main Current Hall Sensing</t>
+  </si>
+  <si>
+    <t>load: typical (A)</t>
+  </si>
+  <si>
+    <t>load: max (A)</t>
+  </si>
+  <si>
+    <t>quiescent load: typical (A)</t>
+  </si>
+  <si>
+    <t>quiescent load: max (A)</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>swapped for 48 pin Q1 mcu</t>
+  </si>
+  <si>
+    <t>notes for future itterations</t>
+  </si>
+  <si>
+    <t>maybe add another onboard relay to control precharge, use MCHS to determine when precharge done/ for now we can just send CAN to the motec</t>
+  </si>
+  <si>
+    <t>swapped IL relay 12v  for 24v</t>
+  </si>
+  <si>
+    <t>U102</t>
   </si>
 </sst>
 </file>
@@ -724,7 +774,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,8 +787,20 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -787,11 +849,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -814,20 +955,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -841,6 +1014,94 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -921,6 +1182,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3CA6A1A-1FD3-48BF-BCF8-90408D82F5F9}" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="7">
+  <autoFilter ref="A1:G3" xr:uid="{B3CA6A1A-1FD3-48BF-BCF8-90408D82F5F9}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F176D1B1-93A9-4FA3-9B13-4D1FB62C21AE}" name="sheet name"/>
+    <tableColumn id="2" xr3:uid="{EE80E7F9-AF23-49F4-943C-5BDA0C2DD776}" name="designator"/>
+    <tableColumn id="3" xr3:uid="{A5946CA3-79A2-4891-BEA3-782B6CE1AAF4}" name="load: typical (A)" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{F1B2DA7A-1733-4CED-911F-2548B461F4B4}" name="load: max (A)" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{FC4198F1-9F4C-462F-A1EC-84FC5B0E5DA5}" name="quiescent load: typical (A)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{4AE8A94A-AE32-4F27-9526-6334655412FD}" name="quiescent load: max (A)" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B9D254ED-3403-48E7-86C6-D472AEB43A1C}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1102,7 +1379,7 @@
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1388,7 @@
     <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
     <col min="9" max="12" width="9.140625" style="1"/>
@@ -1119,7 +1396,7 @@
     <col min="14" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
     <col min="16" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="26.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="123" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1141,11 +1418,11 @@
       <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
       <c r="S1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1729,8 +2006,8 @@
       <c r="D25" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
       <c r="G25" s="3" t="s">
         <v>68</v>
       </c>
@@ -1757,8 +2034,8 @@
       <c r="D26" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
       <c r="G26" s="3" t="s">
         <v>77</v>
       </c>
@@ -1789,8 +2066,8 @@
       <c r="D27" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
       <c r="G27" s="3" t="s">
         <v>100</v>
       </c>
@@ -1821,8 +2098,8 @@
       <c r="D28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="3" t="s">
         <v>103</v>
       </c>
@@ -1850,8 +2127,8 @@
       <c r="D29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="3" t="s">
         <v>88</v>
       </c>
@@ -1879,8 +2156,8 @@
       <c r="D30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="3" t="s">
         <v>90</v>
       </c>
@@ -1986,10 +2263,10 @@
       <c r="D35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F35" s="8"/>
+      <c r="F35" s="10"/>
       <c r="G35" s="3" t="s">
         <v>104</v>
       </c>
@@ -2017,10 +2294,10 @@
       <c r="D36" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F36" s="8"/>
+      <c r="F36" s="10"/>
       <c r="G36" s="3" t="s">
         <v>109</v>
       </c>
@@ -2048,10 +2325,10 @@
       <c r="D37" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F37" s="8"/>
+      <c r="F37" s="10"/>
       <c r="G37" s="3" t="s">
         <v>81</v>
       </c>
@@ -2079,10 +2356,10 @@
       <c r="D38" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F38" s="8"/>
+      <c r="F38" s="10"/>
       <c r="G38" s="3" t="s">
         <v>85</v>
       </c>
@@ -2110,8 +2387,8 @@
       <c r="D39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
       <c r="G39" s="3" t="s">
         <v>122</v>
       </c>
@@ -2139,8 +2416,8 @@
       <c r="D40" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
       <c r="G40" s="3" t="s">
         <v>36</v>
       </c>
@@ -2168,8 +2445,8 @@
       <c r="D41" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
       <c r="G41" s="3" t="s">
         <v>43</v>
       </c>
@@ -2197,8 +2474,8 @@
       <c r="D42" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
       <c r="G42" s="3" t="s">
         <v>117</v>
       </c>
@@ -2226,8 +2503,8 @@
       <c r="D43" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
       <c r="G43" s="3" t="s">
         <v>129</v>
       </c>
@@ -2255,8 +2532,8 @@
       <c r="D44" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
       <c r="G44" s="3" t="s">
         <v>124</v>
       </c>
@@ -2284,8 +2561,8 @@
       <c r="D45" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
       <c r="G45" s="3" t="s">
         <v>93</v>
       </c>
@@ -2313,10 +2590,10 @@
       <c r="D46" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="F46" s="8"/>
+      <c r="F46" s="10"/>
       <c r="G46" s="3" t="s">
         <v>151</v>
       </c>
@@ -2344,10 +2621,10 @@
       <c r="D47" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E47" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="F47" s="8"/>
+      <c r="F47" s="10"/>
       <c r="G47" s="3" t="s">
         <v>151</v>
       </c>
@@ -2375,10 +2652,10 @@
       <c r="D48" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F48" s="10"/>
       <c r="G48" s="3" t="s">
         <v>151</v>
       </c>
@@ -2406,8 +2683,8 @@
       <c r="D49" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
       <c r="G49" s="3" t="s">
         <v>96</v>
       </c>
@@ -2435,10 +2712,10 @@
       <c r="D50" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="F50" s="8"/>
+      <c r="F50" s="10"/>
       <c r="G50" s="3" t="s">
         <v>151</v>
       </c>
@@ -2466,10 +2743,10 @@
       <c r="D51" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E51" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="F51" s="8"/>
+      <c r="F51" s="10"/>
       <c r="G51" s="3" t="s">
         <v>166</v>
       </c>
@@ -2497,8 +2774,8 @@
       <c r="D52" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
       <c r="G52" s="3" t="s">
         <v>169</v>
       </c>
@@ -2526,8 +2803,8 @@
       <c r="D53" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
       <c r="G53" s="3" t="s">
         <v>162</v>
       </c>
@@ -2555,8 +2832,8 @@
       <c r="D54" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
       <c r="G54" s="3" t="s">
         <v>160</v>
       </c>
@@ -2576,8 +2853,8 @@
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="L55" s="3" t="s">
@@ -2593,8 +2870,8 @@
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="L56" s="3" t="s">
@@ -2610,8 +2887,8 @@
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="L57" s="3" t="s">
@@ -2627,8 +2904,8 @@
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="L58" s="3" t="s">
@@ -2712,6 +2989,50 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:F34"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:A5"/>
@@ -2721,58 +3042,14 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:F34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
   </mergeCells>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576 K3">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"n/a"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2787,103 +3064,244 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82506FE1-B017-4B5D-A74A-A8C038FEF2D3}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="111.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
-      <c r="C3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>195</v>
-      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>195</v>
-      </c>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>195</v>
-      </c>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>195</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>194</v>
       </c>
-      <c r="C8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>195</v>
-      </c>
       <c r="B10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>200</v>
-      </c>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>201</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657085C4-1509-4EE7-BF85-5FAE77085CAD}">
+  <dimension ref="A1:U14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="J1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="16"/>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="J3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T12" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R13" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="S13" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="T13" s="11"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T14" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{BFA120B5-3371-45B8-85D7-4B1D8EF2B096}">
+      <formula1>$J:$J</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6560E66A-5941-4854-8E8F-0C87288305BB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
masterbaord schematic nad layout updated for v2
</commit_message>
<xml_diff>
--- a/hardware/MasterBoard_A/Meta MasterBoard A.xlsx
+++ b/hardware/MasterBoard_A/Meta MasterBoard A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\BeeMS\hardware\MasterBoard_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E56E70-1431-4A57-9DC9-1D3390E70CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11A773B-0DE1-4758-AD27-7DBBD24BA3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{4093912D-66FD-41A9-9A54-7EA13A7B271E}"/>
   </bookViews>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="334">
   <si>
     <t>last updated</t>
   </si>
@@ -1150,6 +1150,9 @@
   </si>
   <si>
     <t>use this deticated isolated can transceiver : https://www.mouser.com/ProductDetail/Texas-Instruments/ISO1042DWV?qs=qSfuJ%252Bfl%2Fd6fIgLDsh3Gaw%3D%3D</t>
+  </si>
+  <si>
+    <t>Q502 on hrlv is failing. The BC diode allows power to C which then the gets passed to E.</t>
   </si>
 </sst>
 </file>
@@ -4496,7 +4499,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82506FE1-B017-4B5D-A74A-A8C038FEF2D3}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
@@ -4722,6 +4725,11 @@
     <row r="35" spans="2:2">
       <c r="B35" t="s">
         <v>332</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>